<commit_message>
Added new datasheet - Catalog
</commit_message>
<xml_diff>
--- a/src/test/resources/datasheets/SampleTest.xlsx
+++ b/src/test/resources/datasheets/SampleTest.xlsx
@@ -11,7 +11,6 @@
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <oleSize ref="A1:O19"/>
 </workbook>
 </file>
 
@@ -860,13 +859,20 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.140625" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="4" max="4" width="33" customWidth="1"/>
+    <col min="5" max="5" width="21" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" customWidth="1"/>
+    <col min="7" max="7" width="17" customWidth="1"/>
+    <col min="8" max="8" width="22.7109375" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">

</xml_diff>